<commit_message>
SIB: fix nickel emissions
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-batteries-SIB.xlsx
+++ b/premise/data/additional_inventories/lci-batteries-SIB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahnme_a\PycharmProjects\premise\premise\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18974D2D-D0D8-4C99-B853-578B8B4A6F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB1C9EC-68A4-4419-BFEE-3497B1615209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="sodium-ion batteries" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sodium-ion batteries'!$A$1:$K$479</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sodium-ion batteries'!$A$1:$K$480</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="264">
   <si>
     <t>Database</t>
   </si>
@@ -864,6 +864,15 @@
   </si>
   <si>
     <t>nickel carbonate, anhydrous, at plant</t>
+  </si>
+  <si>
+    <t>Original inventory assumed no further wastewater treatment</t>
+  </si>
+  <si>
+    <t>Original inventory: 0.0127kg | This value was modified to align with industrial wastewater regulations</t>
+  </si>
+  <si>
+    <t>Original inventory: 0.013kg | This value was modified to align with industrial wastewater regulations</t>
   </si>
 </sst>
 </file>
@@ -937,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -950,6 +959,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K515"/>
+  <dimension ref="A1:K516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A503" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B526" sqref="B526"/>
+    <sheetView tabSelected="1" topLeftCell="A382" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G404" sqref="G404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7356,7 +7366,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>27</v>
       </c>
@@ -7379,7 +7389,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>150</v>
       </c>
@@ -7402,7 +7412,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>1</v>
       </c>
@@ -7410,7 +7420,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>2</v>
       </c>
@@ -7418,7 +7428,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>227</v>
       </c>
@@ -7426,7 +7436,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>3</v>
       </c>
@@ -7434,7 +7444,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>5</v>
       </c>
@@ -7442,7 +7452,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>6</v>
       </c>
@@ -7450,7 +7460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>216</v>
       </c>
@@ -7458,12 +7468,12 @@
         <v>220</v>
       </c>
     </row>
-    <row r="395" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>9</v>
       </c>
@@ -7488,8 +7498,12 @@
       <c r="H396" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I396" t="s">
+        <v>2</v>
+      </c>
+      <c r="K396" s="12"/>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>69</v>
       </c>
@@ -7509,7 +7523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>14</v>
       </c>
@@ -7529,12 +7543,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>259</v>
       </c>
-      <c r="B399">
-        <v>1.2999999999999999E-2</v>
+      <c r="B399" s="12">
+        <v>3.9999999999999998E-7</v>
       </c>
       <c r="C399" t="s">
         <v>31</v>
@@ -7548,13 +7562,16 @@
       <c r="G399" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I399" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>167</v>
       </c>
-      <c r="B400">
-        <v>1.2699999999999999E-2</v>
+      <c r="B400" s="12">
+        <v>3.9999999999999998E-7</v>
       </c>
       <c r="C400" t="s">
         <v>31</v>
@@ -7568,8 +7585,11 @@
       <c r="G400" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I400" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="401" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>151</v>
       </c>
@@ -7589,7 +7609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>152</v>
       </c>
@@ -7609,7 +7629,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>199</v>
       </c>
@@ -7632,7 +7652,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>153</v>
       </c>
@@ -7655,7 +7675,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>101</v>
       </c>
@@ -7678,7 +7698,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>127</v>
       </c>
@@ -7701,7 +7721,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>25</v>
       </c>
@@ -7724,7 +7744,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>81</v>
       </c>
@@ -7747,7 +7767,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>27</v>
       </c>
@@ -7770,7 +7790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>85</v>
       </c>
@@ -7793,111 +7813,115 @@
         <v>66</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A412" s="1" t="s">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>55</v>
+      </c>
+      <c r="B411">
+        <f>-B410/1000</f>
+        <v>-7.980000000000001E-3</v>
+      </c>
+      <c r="C411" t="s">
+        <v>165</v>
+      </c>
+      <c r="D411" t="s">
+        <v>56</v>
+      </c>
+      <c r="E411" t="s">
+        <v>57</v>
+      </c>
+      <c r="G411" t="s">
+        <v>19</v>
+      </c>
+      <c r="H411" t="s">
+        <v>58</v>
+      </c>
+      <c r="I411" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A413" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B412" s="1" t="s">
+      <c r="B413" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A413" t="s">
+    <row r="414" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
         <v>2</v>
       </c>
-      <c r="B413" t="s">
+      <c r="B414" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A414" t="s">
+    <row r="415" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
         <v>3</v>
       </c>
-      <c r="B414" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A415" t="s">
+      <c r="B415" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="416" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
         <v>5</v>
       </c>
-      <c r="B415" t="s">
+      <c r="B416" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A416" t="s">
-        <v>6</v>
-      </c>
-      <c r="B416" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="417" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
+        <v>6</v>
+      </c>
+      <c r="B417" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
         <v>216</v>
       </c>
-      <c r="B417" t="s">
+      <c r="B418" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="418" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A418" s="1" t="s">
+    <row r="419" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A419" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A419" t="s">
-        <v>9</v>
-      </c>
-      <c r="B419" t="s">
-        <v>10</v>
-      </c>
-      <c r="C419" t="s">
-        <v>11</v>
-      </c>
-      <c r="D419" t="s">
-        <v>3</v>
-      </c>
-      <c r="E419" t="s">
-        <v>6</v>
-      </c>
-      <c r="F419" t="s">
-        <v>13</v>
-      </c>
-      <c r="G419" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>201</v>
-      </c>
-      <c r="B420">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B420" t="s">
+        <v>10</v>
       </c>
       <c r="C420" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="D420" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E420" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F420" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G420" t="s">
-        <v>202</v>
+        <v>5</v>
       </c>
     </row>
     <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B421">
-        <v>0.13180285392336399</v>
+        <v>1</v>
       </c>
       <c r="C421" t="s">
         <v>164</v>
@@ -7909,24 +7933,24 @@
         <v>7</v>
       </c>
       <c r="F421" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G421" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="B422">
-        <v>0.38852820840736102</v>
+        <v>0.13180285392336399</v>
       </c>
       <c r="C422" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D422" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E422" t="s">
         <v>7</v>
@@ -7935,15 +7959,15 @@
         <v>19</v>
       </c>
       <c r="G422" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B423">
-        <v>0.47966893766927499</v>
+        <v>0.38852820840736102</v>
       </c>
       <c r="C423" t="s">
         <v>165</v>
@@ -7958,38 +7982,38 @@
         <v>19</v>
       </c>
       <c r="G423" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="424" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="B424">
-        <v>0.1</v>
+        <v>0.47966893766927499</v>
       </c>
       <c r="C424" t="s">
         <v>165</v>
       </c>
       <c r="D424" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E424" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F424" t="s">
         <v>19</v>
       </c>
       <c r="G424" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
     </row>
     <row r="425" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B425">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="C425" t="s">
         <v>165</v>
@@ -8004,271 +8028,270 @@
         <v>19</v>
       </c>
       <c r="G425" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>27</v>
+      </c>
+      <c r="B426">
+        <v>0.6</v>
+      </c>
+      <c r="C426" t="s">
+        <v>165</v>
+      </c>
+      <c r="D426" t="s">
+        <v>4</v>
+      </c>
+      <c r="E426" t="s">
+        <v>24</v>
+      </c>
+      <c r="F426" t="s">
+        <v>19</v>
+      </c>
+      <c r="G426" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A427" s="1" t="s">
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A428" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B427" s="1" t="s">
+      <c r="B428" s="1" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A428" t="s">
-        <v>3</v>
-      </c>
-      <c r="B428" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="429" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B429" t="s">
-        <v>226</v>
+        <v>4</v>
       </c>
     </row>
     <row r="430" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B430" t="s">
-        <v>28</v>
+        <v>226</v>
       </c>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B431" t="s">
-        <v>223</v>
+        <v>28</v>
       </c>
     </row>
     <row r="432" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B432" t="s">
-        <v>7</v>
+        <v>223</v>
       </c>
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
+        <v>6</v>
+      </c>
+      <c r="B433" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
         <v>216</v>
       </c>
-      <c r="B433" t="s">
+      <c r="B434" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A434" s="1" t="s">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A435" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B434" s="1"/>
-      <c r="C434" s="1"/>
-      <c r="D434" s="1"/>
-      <c r="E434" s="1"/>
-      <c r="F434" s="1"/>
-      <c r="G434" s="1"/>
-      <c r="H434" s="1"/>
-      <c r="I434" s="1"/>
-      <c r="J434" s="1"/>
-      <c r="K434" s="1"/>
-    </row>
-    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A435" t="s">
-        <v>9</v>
-      </c>
-      <c r="B435" t="s">
-        <v>10</v>
-      </c>
-      <c r="C435" t="s">
-        <v>11</v>
-      </c>
-      <c r="D435" t="s">
-        <v>3</v>
-      </c>
-      <c r="E435" t="s">
-        <v>6</v>
-      </c>
-      <c r="F435" t="s">
-        <v>13</v>
-      </c>
-      <c r="G435" t="s">
-        <v>5</v>
-      </c>
+      <c r="B435" s="1"/>
+      <c r="C435" s="1"/>
+      <c r="D435" s="1"/>
+      <c r="E435" s="1"/>
+      <c r="F435" s="1"/>
+      <c r="G435" s="1"/>
+      <c r="H435" s="1"/>
+      <c r="I435" s="1"/>
+      <c r="J435" s="1"/>
+      <c r="K435" s="1"/>
     </row>
     <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>203</v>
-      </c>
-      <c r="B436">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B436" t="s">
+        <v>10</v>
       </c>
       <c r="C436" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="D436" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E436" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F436" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G436" t="s">
-        <v>226</v>
+        <v>5</v>
       </c>
     </row>
     <row r="437" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
+        <v>203</v>
+      </c>
+      <c r="B437">
+        <v>1</v>
+      </c>
+      <c r="C437" t="s">
+        <v>164</v>
+      </c>
+      <c r="D437" t="s">
+        <v>4</v>
+      </c>
+      <c r="E437" t="s">
+        <v>7</v>
+      </c>
+      <c r="F437" t="s">
+        <v>18</v>
+      </c>
+      <c r="G437" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
         <v>169</v>
       </c>
-      <c r="B437">
+      <c r="B438">
         <f>(1/0.0562)*0.0085612534146254</f>
         <v>0.1523354700111281</v>
       </c>
-      <c r="C437" t="s">
+      <c r="C438" t="s">
         <v>164</v>
       </c>
-      <c r="D437" t="s">
-        <v>4</v>
-      </c>
-      <c r="E437" t="s">
-        <v>7</v>
-      </c>
-      <c r="F437" t="s">
-        <v>19</v>
-      </c>
-      <c r="G437" t="s">
+      <c r="D438" t="s">
+        <v>4</v>
+      </c>
+      <c r="E438" t="s">
+        <v>7</v>
+      </c>
+      <c r="F438" t="s">
+        <v>19</v>
+      </c>
+      <c r="G438" t="s">
         <v>168</v>
       </c>
-      <c r="H437" t="s">
+      <c r="H438" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A438" t="s">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
         <v>183</v>
       </c>
-      <c r="B438">
+      <c r="B439">
         <f>(1/0.0562)*0.0165620491137194</f>
         <v>0.29469838280639504</v>
       </c>
-      <c r="C438" t="s">
+      <c r="C439" t="s">
         <v>164</v>
       </c>
-      <c r="D438" t="s">
-        <v>4</v>
-      </c>
-      <c r="E438" t="s">
-        <v>7</v>
-      </c>
-      <c r="F438" t="s">
-        <v>19</v>
-      </c>
-      <c r="G438" t="s">
+      <c r="D439" t="s">
+        <v>4</v>
+      </c>
+      <c r="E439" t="s">
+        <v>7</v>
+      </c>
+      <c r="F439" t="s">
+        <v>19</v>
+      </c>
+      <c r="G439" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A439" t="s">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
         <v>185</v>
       </c>
-      <c r="B439">
+      <c r="B440">
         <f>(1/0.0562)*0.0209977698868578</f>
         <v>0.37362579869853735</v>
       </c>
-      <c r="C439" t="s">
+      <c r="C440" t="s">
         <v>164</v>
       </c>
-      <c r="D439" t="s">
-        <v>4</v>
-      </c>
-      <c r="E439" t="s">
-        <v>7</v>
-      </c>
-      <c r="F439" t="s">
-        <v>19</v>
-      </c>
-      <c r="G439" t="s">
+      <c r="D440" t="s">
+        <v>4</v>
+      </c>
+      <c r="E440" t="s">
+        <v>7</v>
+      </c>
+      <c r="F440" t="s">
+        <v>19</v>
+      </c>
+      <c r="G440" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A440" t="s">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
         <v>201</v>
       </c>
-      <c r="B440">
+      <c r="B441">
         <f>(1/0.0562)*0.00925252694737966</f>
         <v>0.16463571080746725</v>
       </c>
-      <c r="C440" t="s">
+      <c r="C441" t="s">
         <v>164</v>
       </c>
-      <c r="D440" t="s">
-        <v>4</v>
-      </c>
-      <c r="E440" t="s">
-        <v>7</v>
-      </c>
-      <c r="F440" t="s">
-        <v>19</v>
-      </c>
-      <c r="G440" t="s">
+      <c r="D441" t="s">
+        <v>4</v>
+      </c>
+      <c r="E441" t="s">
+        <v>7</v>
+      </c>
+      <c r="F441" t="s">
+        <v>19</v>
+      </c>
+      <c r="G441" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A441" t="s">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
         <v>86</v>
       </c>
-      <c r="B441">
+      <c r="B442">
         <f>(1/0.0562)*0.000803030859695695</f>
         <v>1.4288805332663612E-2</v>
       </c>
-      <c r="C441" t="s">
-        <v>165</v>
-      </c>
-      <c r="D441" t="s">
+      <c r="C442" t="s">
+        <v>165</v>
+      </c>
+      <c r="D442" t="s">
         <v>21</v>
       </c>
-      <c r="E441" t="s">
-        <v>7</v>
-      </c>
-      <c r="F441" t="s">
-        <v>19</v>
-      </c>
-      <c r="G441" t="s">
+      <c r="E442" t="s">
+        <v>7</v>
+      </c>
+      <c r="F442" t="s">
+        <v>19</v>
+      </c>
+      <c r="G442" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A442" t="s">
-        <v>25</v>
-      </c>
-      <c r="B442">
-        <f>(1/0.0562)*0.103774876494967</f>
-        <v>1.8465280515118683</v>
-      </c>
-      <c r="C442" t="s">
-        <v>165</v>
-      </c>
-      <c r="D442" t="s">
-        <v>4</v>
-      </c>
-      <c r="E442" t="s">
-        <v>26</v>
-      </c>
-      <c r="F442" t="s">
-        <v>19</v>
-      </c>
-      <c r="G442" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="443" spans="1:11" x14ac:dyDescent="0.25">
@@ -8276,281 +8299,281 @@
         <v>25</v>
       </c>
       <c r="B443">
+        <f>(1/0.0562)*0.103774876494967</f>
+        <v>1.8465280515118683</v>
+      </c>
+      <c r="C443" t="s">
+        <v>165</v>
+      </c>
+      <c r="D443" t="s">
+        <v>4</v>
+      </c>
+      <c r="E443" t="s">
+        <v>26</v>
+      </c>
+      <c r="F443" t="s">
+        <v>19</v>
+      </c>
+      <c r="G443" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>25</v>
+      </c>
+      <c r="B444">
         <f>(1/0.0562)*0.133972324705964</f>
         <v>2.3838491940562991</v>
       </c>
-      <c r="C443" t="s">
-        <v>165</v>
-      </c>
-      <c r="D443" t="s">
-        <v>4</v>
-      </c>
-      <c r="E443" t="s">
+      <c r="C444" t="s">
+        <v>165</v>
+      </c>
+      <c r="D444" t="s">
+        <v>4</v>
+      </c>
+      <c r="E444" t="s">
         <v>26</v>
       </c>
-      <c r="F443" t="s">
-        <v>19</v>
-      </c>
-      <c r="G443" t="s">
+      <c r="F444" t="s">
+        <v>19</v>
+      </c>
+      <c r="G444" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A445" s="1" t="s">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A446" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B445" s="1" t="s">
+      <c r="B446" s="1" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A446" t="s">
-        <v>3</v>
-      </c>
-      <c r="B446" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="447" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B447" t="s">
-        <v>226</v>
+        <v>4</v>
       </c>
     </row>
     <row r="448" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B448" t="s">
-        <v>28</v>
+        <v>226</v>
       </c>
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B449" t="s">
-        <v>224</v>
+        <v>28</v>
       </c>
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B450" t="s">
-        <v>7</v>
+        <v>224</v>
       </c>
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
+        <v>6</v>
+      </c>
+      <c r="B451" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
         <v>216</v>
       </c>
-      <c r="B451" t="s">
+      <c r="B452" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A452" s="1" t="s">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A453" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A453" t="s">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
         <v>9</v>
       </c>
-      <c r="B453" t="s">
+      <c r="B454" t="s">
         <v>10</v>
       </c>
-      <c r="C453" t="s">
+      <c r="C454" t="s">
         <v>11</v>
       </c>
-      <c r="D453" t="s">
+      <c r="D454" t="s">
         <v>3</v>
       </c>
-      <c r="E453" t="s">
+      <c r="E454" t="s">
         <v>6</v>
       </c>
-      <c r="F453" t="s">
+      <c r="F454" t="s">
         <v>13</v>
       </c>
-      <c r="G453" t="s">
+      <c r="G454" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="454" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A454" t="s">
+    <row r="455" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
         <v>204</v>
       </c>
-      <c r="B454">
+      <c r="B455">
         <v>1</v>
       </c>
-      <c r="C454" t="s">
+      <c r="C455" t="s">
         <v>164</v>
       </c>
-      <c r="D454" t="s">
-        <v>4</v>
-      </c>
-      <c r="E454" t="s">
-        <v>7</v>
-      </c>
-      <c r="F454" t="s">
+      <c r="D455" t="s">
+        <v>4</v>
+      </c>
+      <c r="E455" t="s">
+        <v>7</v>
+      </c>
+      <c r="F455" t="s">
         <v>18</v>
       </c>
-      <c r="G454" t="s">
+      <c r="G455" t="s">
         <v>226</v>
       </c>
-      <c r="H454"/>
-      <c r="I454"/>
-      <c r="J454"/>
-      <c r="K454"/>
-    </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A455" t="s">
+      <c r="H455"/>
+      <c r="I455"/>
+      <c r="J455"/>
+      <c r="K455"/>
+    </row>
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
         <v>169</v>
       </c>
-      <c r="B455">
+      <c r="B456">
         <f>(1/0.053177)*0.0085612534146254</f>
         <v>0.1609954193471877</v>
       </c>
-      <c r="C455" t="s">
+      <c r="C456" t="s">
         <v>164</v>
       </c>
-      <c r="D455" t="s">
-        <v>4</v>
-      </c>
-      <c r="E455" t="s">
-        <v>7</v>
-      </c>
-      <c r="F455" t="s">
-        <v>19</v>
-      </c>
-      <c r="G455" t="s">
+      <c r="D456" t="s">
+        <v>4</v>
+      </c>
+      <c r="E456" t="s">
+        <v>7</v>
+      </c>
+      <c r="F456" t="s">
+        <v>19</v>
+      </c>
+      <c r="G456" t="s">
         <v>168</v>
       </c>
-      <c r="H455" t="s">
+      <c r="H456" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A456" t="s">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
         <v>172</v>
       </c>
-      <c r="B456">
+      <c r="B457">
         <f>(1/0.053177)*0.0130181682473286</f>
         <v>0.24480824881675539</v>
       </c>
-      <c r="C456" t="s">
+      <c r="C457" t="s">
         <v>164</v>
       </c>
-      <c r="D456" t="s">
-        <v>4</v>
-      </c>
-      <c r="E456" t="s">
-        <v>7</v>
-      </c>
-      <c r="F456" t="s">
-        <v>19</v>
-      </c>
-      <c r="G456" t="s">
+      <c r="D457" t="s">
+        <v>4</v>
+      </c>
+      <c r="E457" t="s">
+        <v>7</v>
+      </c>
+      <c r="F457" t="s">
+        <v>19</v>
+      </c>
+      <c r="G457" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A457" t="s">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
         <v>188</v>
       </c>
-      <c r="B457">
+      <c r="B458">
         <f>(1/0.053177)*0.0216120622410464</f>
         <v>0.40641747825274838</v>
       </c>
-      <c r="C457" t="s">
+      <c r="C458" t="s">
         <v>164</v>
       </c>
-      <c r="D457" t="s">
-        <v>4</v>
-      </c>
-      <c r="E457" t="s">
-        <v>7</v>
-      </c>
-      <c r="F457" t="s">
-        <v>19</v>
-      </c>
-      <c r="G457" t="s">
+      <c r="D458" t="s">
+        <v>4</v>
+      </c>
+      <c r="E458" t="s">
+        <v>7</v>
+      </c>
+      <c r="F458" t="s">
+        <v>19</v>
+      </c>
+      <c r="G458" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A458" t="s">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
         <v>201</v>
       </c>
-      <c r="B458">
+      <c r="B459">
         <f>(1/0.053177)*0.00934397682507009</f>
         <v>0.17571462897625084</v>
       </c>
-      <c r="C458" t="s">
+      <c r="C459" t="s">
         <v>164</v>
       </c>
-      <c r="D458" t="s">
-        <v>4</v>
-      </c>
-      <c r="E458" t="s">
-        <v>7</v>
-      </c>
-      <c r="F458" t="s">
-        <v>19</v>
-      </c>
-      <c r="G458" t="s">
+      <c r="D459" t="s">
+        <v>4</v>
+      </c>
+      <c r="E459" t="s">
+        <v>7</v>
+      </c>
+      <c r="F459" t="s">
+        <v>19</v>
+      </c>
+      <c r="G459" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A459" t="s">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
         <v>86</v>
       </c>
-      <c r="B459">
+      <c r="B460">
         <f>(1/0.053177)*0.000642010008010976</f>
         <v>1.2073076856742127E-2</v>
       </c>
-      <c r="C459" t="s">
-        <v>165</v>
-      </c>
-      <c r="D459" t="s">
+      <c r="C460" t="s">
+        <v>165</v>
+      </c>
+      <c r="D460" t="s">
         <v>21</v>
       </c>
-      <c r="E459" t="s">
-        <v>7</v>
-      </c>
-      <c r="F459" t="s">
-        <v>19</v>
-      </c>
-      <c r="G459" t="s">
+      <c r="E460" t="s">
+        <v>7</v>
+      </c>
+      <c r="F460" t="s">
+        <v>19</v>
+      </c>
+      <c r="G460" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A460" t="s">
-        <v>25</v>
-      </c>
-      <c r="B460">
-        <f>(1/0.053177)*0.104800563836034</f>
-        <v>1.9707874426168082</v>
-      </c>
-      <c r="C460" t="s">
-        <v>165</v>
-      </c>
-      <c r="D460" t="s">
-        <v>4</v>
-      </c>
-      <c r="E460" t="s">
-        <v>26</v>
-      </c>
-      <c r="F460" t="s">
-        <v>19</v>
-      </c>
-      <c r="G460" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.25">
@@ -8558,302 +8581,299 @@
         <v>25</v>
       </c>
       <c r="B461">
+        <f>(1/0.053177)*0.104800563836034</f>
+        <v>1.9707874426168082</v>
+      </c>
+      <c r="C461" t="s">
+        <v>165</v>
+      </c>
+      <c r="D461" t="s">
+        <v>4</v>
+      </c>
+      <c r="E461" t="s">
+        <v>26</v>
+      </c>
+      <c r="F461" t="s">
+        <v>19</v>
+      </c>
+      <c r="G461" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="462" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>25</v>
+      </c>
+      <c r="B462">
         <f>(1/0.053177)*0.125938218719691</f>
         <v>2.3682836323916541</v>
       </c>
-      <c r="C461" t="s">
-        <v>165</v>
-      </c>
-      <c r="D461" t="s">
-        <v>4</v>
-      </c>
-      <c r="E461" t="s">
+      <c r="C462" t="s">
+        <v>165</v>
+      </c>
+      <c r="D462" t="s">
+        <v>4</v>
+      </c>
+      <c r="E462" t="s">
         <v>26</v>
       </c>
-      <c r="F461" t="s">
-        <v>19</v>
-      </c>
-      <c r="G461" t="s">
+      <c r="F462" t="s">
+        <v>19</v>
+      </c>
+      <c r="G462" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A463" s="1" t="s">
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A464" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B463" s="1" t="s">
+      <c r="B464" s="1" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A464" t="s">
-        <v>3</v>
-      </c>
-      <c r="B464" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="465" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B465" t="s">
-        <v>226</v>
+        <v>4</v>
       </c>
     </row>
     <row r="466" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B466" t="s">
-        <v>28</v>
+        <v>226</v>
       </c>
     </row>
     <row r="467" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B467" t="s">
-        <v>225</v>
+        <v>28</v>
       </c>
     </row>
     <row r="468" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B468" t="s">
-        <v>7</v>
+        <v>225</v>
       </c>
     </row>
     <row r="469" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
+        <v>6</v>
+      </c>
+      <c r="B469" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
         <v>216</v>
       </c>
-      <c r="B469" t="s">
+      <c r="B470" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A470" s="1" t="s">
+    <row r="471" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A471" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B470" s="1"/>
-      <c r="C470" s="1"/>
-      <c r="D470" s="1"/>
-      <c r="E470" s="1"/>
-      <c r="F470" s="1"/>
-      <c r="G470" s="1"/>
-      <c r="H470" s="1"/>
-      <c r="I470" s="1"/>
-      <c r="J470" s="1"/>
-      <c r="K470" s="1"/>
-    </row>
-    <row r="471" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
-        <v>9</v>
-      </c>
-      <c r="B471" t="s">
-        <v>10</v>
-      </c>
-      <c r="C471" t="s">
-        <v>11</v>
-      </c>
-      <c r="D471" t="s">
-        <v>3</v>
-      </c>
-      <c r="E471" t="s">
-        <v>6</v>
-      </c>
-      <c r="F471" t="s">
-        <v>13</v>
-      </c>
-      <c r="G471" t="s">
-        <v>5</v>
-      </c>
-      <c r="H471" t="s">
-        <v>2</v>
-      </c>
+      <c r="B471" s="1"/>
+      <c r="C471" s="1"/>
+      <c r="D471" s="1"/>
+      <c r="E471" s="1"/>
+      <c r="F471" s="1"/>
+      <c r="G471" s="1"/>
+      <c r="H471" s="1"/>
+      <c r="I471" s="1"/>
+      <c r="J471" s="1"/>
+      <c r="K471" s="1"/>
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>205</v>
-      </c>
-      <c r="B472">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B472" t="s">
+        <v>10</v>
       </c>
       <c r="C472" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="D472" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E472" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F472" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G472" t="s">
-        <v>226</v>
+        <v>5</v>
+      </c>
+      <c r="H472" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="473" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
+        <v>205</v>
+      </c>
+      <c r="B473">
+        <v>1</v>
+      </c>
+      <c r="C473" t="s">
+        <v>164</v>
+      </c>
+      <c r="D473" t="s">
+        <v>4</v>
+      </c>
+      <c r="E473" t="s">
+        <v>7</v>
+      </c>
+      <c r="F473" t="s">
+        <v>18</v>
+      </c>
+      <c r="G473" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="474" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
         <v>169</v>
       </c>
-      <c r="B473">
+      <c r="B474">
         <f>(1/0.045)*0.0085612534146254</f>
         <v>0.19025007588056442</v>
       </c>
-      <c r="C473" t="s">
+      <c r="C474" t="s">
         <v>164</v>
       </c>
-      <c r="D473" t="s">
-        <v>4</v>
-      </c>
-      <c r="E473" t="s">
-        <v>7</v>
-      </c>
-      <c r="F473" t="s">
-        <v>19</v>
-      </c>
-      <c r="G473" t="s">
+      <c r="D474" t="s">
+        <v>4</v>
+      </c>
+      <c r="E474" t="s">
+        <v>7</v>
+      </c>
+      <c r="F474" t="s">
+        <v>19</v>
+      </c>
+      <c r="G474" t="s">
         <v>168</v>
       </c>
-      <c r="H473" t="s">
+      <c r="H474" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="474" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A474" t="s">
+    <row r="475" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
         <v>192</v>
       </c>
-      <c r="B474">
+      <c r="B475">
         <f>(1/0.045)*0.0109585812086088</f>
         <v>0.24352402685797334</v>
       </c>
-      <c r="C474" t="s">
+      <c r="C475" t="s">
         <v>164</v>
       </c>
-      <c r="D474" t="s">
-        <v>4</v>
-      </c>
-      <c r="E474" t="s">
-        <v>7</v>
-      </c>
-      <c r="F474" t="s">
-        <v>19</v>
-      </c>
-      <c r="G474" t="s">
+      <c r="D475" t="s">
+        <v>4</v>
+      </c>
+      <c r="E475" t="s">
+        <v>7</v>
+      </c>
+      <c r="F475" t="s">
+        <v>19</v>
+      </c>
+      <c r="G475" t="s">
         <v>193</v>
       </c>
-      <c r="H474" t="s">
+      <c r="H475" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="475" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A475" t="s">
+    <row r="476" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
         <v>195</v>
       </c>
-      <c r="B475">
+      <c r="B476">
         <f>(1/0.045)*0.0154881832669088</f>
         <v>0.34418185037575111</v>
       </c>
-      <c r="C475" t="s">
+      <c r="C476" t="s">
         <v>164</v>
       </c>
-      <c r="D475" t="s">
-        <v>4</v>
-      </c>
-      <c r="E475" t="s">
-        <v>7</v>
-      </c>
-      <c r="F475" t="s">
-        <v>19</v>
-      </c>
-      <c r="G475" t="s">
+      <c r="D476" t="s">
+        <v>4</v>
+      </c>
+      <c r="E476" t="s">
+        <v>7</v>
+      </c>
+      <c r="F476" t="s">
+        <v>19</v>
+      </c>
+      <c r="G476" t="s">
         <v>196</v>
       </c>
-      <c r="H475" t="s">
+      <c r="H476" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="476" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A476" t="s">
+    <row r="477" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
         <v>201</v>
       </c>
-      <c r="B476">
+      <c r="B477">
         <f>(1/0.045)*0.00937223587605556</f>
         <v>0.20827190835679019</v>
       </c>
-      <c r="C476" t="s">
+      <c r="C477" t="s">
         <v>164</v>
       </c>
-      <c r="D476" t="s">
-        <v>4</v>
-      </c>
-      <c r="E476" t="s">
-        <v>7</v>
-      </c>
-      <c r="F476" t="s">
-        <v>19</v>
-      </c>
-      <c r="G476" t="s">
+      <c r="D477" t="s">
+        <v>4</v>
+      </c>
+      <c r="E477" t="s">
+        <v>7</v>
+      </c>
+      <c r="F477" t="s">
+        <v>19</v>
+      </c>
+      <c r="G477" t="s">
         <v>202</v>
       </c>
-      <c r="H476" t="s">
+      <c r="H477" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="477" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A477" t="s">
+    <row r="478" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
         <v>86</v>
       </c>
-      <c r="B477">
+      <c r="B478">
         <f>(1/0.045)*0.000592324289244388</f>
         <v>1.3162761983208621E-2</v>
       </c>
-      <c r="C477" t="s">
-        <v>165</v>
-      </c>
-      <c r="D477" t="s">
+      <c r="C478" t="s">
+        <v>165</v>
+      </c>
+      <c r="D478" t="s">
         <v>21</v>
       </c>
-      <c r="E477" t="s">
-        <v>7</v>
-      </c>
-      <c r="F477" t="s">
-        <v>19</v>
-      </c>
-      <c r="G477" t="s">
+      <c r="E478" t="s">
+        <v>7</v>
+      </c>
+      <c r="F478" t="s">
+        <v>19</v>
+      </c>
+      <c r="G478" t="s">
         <v>163</v>
-      </c>
-      <c r="H477" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="478" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A478" t="s">
-        <v>25</v>
-      </c>
-      <c r="B478">
-        <f>(1/0.045)*0.105117512875205</f>
-        <v>2.3359447305601111</v>
-      </c>
-      <c r="C478" t="s">
-        <v>165</v>
-      </c>
-      <c r="D478" t="s">
-        <v>4</v>
-      </c>
-      <c r="E478" t="s">
-        <v>26</v>
-      </c>
-      <c r="F478" t="s">
-        <v>19</v>
-      </c>
-      <c r="G478" t="s">
-        <v>62</v>
       </c>
       <c r="H478" t="s">
         <v>217</v>
@@ -8864,428 +8884,433 @@
         <v>25</v>
       </c>
       <c r="B479">
+        <f>(1/0.045)*0.105117512875205</f>
+        <v>2.3359447305601111</v>
+      </c>
+      <c r="C479" t="s">
+        <v>165</v>
+      </c>
+      <c r="D479" t="s">
+        <v>4</v>
+      </c>
+      <c r="E479" t="s">
+        <v>26</v>
+      </c>
+      <c r="F479" t="s">
+        <v>19</v>
+      </c>
+      <c r="G479" t="s">
+        <v>62</v>
+      </c>
+      <c r="H479" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="480" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>25</v>
+      </c>
+      <c r="B480">
         <f>(1/0.045)*0.0936148404555879</f>
         <v>2.0803297879019533</v>
       </c>
-      <c r="C479" t="s">
-        <v>165</v>
-      </c>
-      <c r="D479" t="s">
-        <v>4</v>
-      </c>
-      <c r="E479" t="s">
+      <c r="C480" t="s">
+        <v>165</v>
+      </c>
+      <c r="D480" t="s">
+        <v>4</v>
+      </c>
+      <c r="E480" t="s">
         <v>26</v>
       </c>
-      <c r="F479" t="s">
-        <v>19</v>
-      </c>
-      <c r="G479" t="s">
+      <c r="F480" t="s">
+        <v>19</v>
+      </c>
+      <c r="G480" t="s">
         <v>62</v>
       </c>
-      <c r="H479" t="s">
+      <c r="H480" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="481" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A481" s="2" t="s">
+    <row r="482" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A482" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B481" s="2" t="s">
+      <c r="B482" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="482" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A482" s="3" t="s">
+    <row r="483" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A483" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B482" s="3" t="s">
+      <c r="B483" s="3" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="483" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A483" t="s">
-        <v>3</v>
-      </c>
-      <c r="B483" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="484" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>230</v>
-      </c>
-      <c r="B484">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B484" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="485" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>5</v>
-      </c>
-      <c r="B485" t="s">
-        <v>254</v>
+        <v>230</v>
+      </c>
+      <c r="B485">
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B486" t="s">
-        <v>7</v>
+        <v>254</v>
       </c>
     </row>
     <row r="487" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
+        <v>6</v>
+      </c>
+      <c r="B487" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="488" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
         <v>216</v>
       </c>
-      <c r="B487" t="s">
+      <c r="B488" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="488" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A488" s="1" t="s">
+    <row r="489" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A489" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="489" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A489" t="s">
-        <v>9</v>
-      </c>
-      <c r="B489" t="s">
-        <v>10</v>
-      </c>
-      <c r="C489" t="s">
-        <v>6</v>
-      </c>
-      <c r="D489" t="s">
-        <v>12</v>
-      </c>
-      <c r="E489" t="s">
-        <v>3</v>
-      </c>
-      <c r="F489" t="s">
-        <v>13</v>
-      </c>
-      <c r="G489" t="s">
-        <v>5</v>
-      </c>
-      <c r="H489" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="490" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>238</v>
-      </c>
-      <c r="B490">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B490" t="s">
+        <v>10</v>
       </c>
       <c r="C490" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D490" t="s">
+        <v>12</v>
       </c>
       <c r="E490" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F490" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G490" t="s">
-        <v>254</v>
+        <v>5</v>
+      </c>
+      <c r="H490" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="491" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
+        <v>238</v>
+      </c>
+      <c r="B491">
+        <v>1</v>
+      </c>
+      <c r="C491" t="s">
+        <v>7</v>
+      </c>
+      <c r="E491" t="s">
+        <v>21</v>
+      </c>
+      <c r="F491" t="s">
+        <v>18</v>
+      </c>
+      <c r="G491" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="492" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
         <v>203</v>
       </c>
-      <c r="B491" s="4">
+      <c r="B492" s="4">
         <f>408*0.046/24.971</f>
         <v>0.75159184654198874</v>
       </c>
-      <c r="C491" t="s">
-        <v>7</v>
-      </c>
-      <c r="E491" t="s">
-        <v>4</v>
-      </c>
-      <c r="F491" t="s">
-        <v>19</v>
-      </c>
-      <c r="G491" t="s">
+      <c r="C492" t="s">
+        <v>7</v>
+      </c>
+      <c r="E492" t="s">
+        <v>4</v>
+      </c>
+      <c r="F492" t="s">
+        <v>19</v>
+      </c>
+      <c r="G492" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="492" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A492" t="s">
+    <row r="493" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
         <v>239</v>
       </c>
-      <c r="B492" s="4">
+      <c r="B493" s="4">
         <f>0.275/24.971</f>
         <v>1.1012774818789798E-2</v>
       </c>
-      <c r="C492" t="s">
-        <v>7</v>
-      </c>
-      <c r="E492" t="s">
+      <c r="C493" t="s">
+        <v>7</v>
+      </c>
+      <c r="E493" t="s">
         <v>21</v>
       </c>
-      <c r="F492" t="s">
-        <v>19</v>
-      </c>
-      <c r="G492" t="s">
+      <c r="F493" t="s">
+        <v>19</v>
+      </c>
+      <c r="G493" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="493" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A493" t="s">
+    <row r="494" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
         <v>241</v>
       </c>
-      <c r="B493" s="4">
+      <c r="B494" s="4">
         <f>0.593/24.971</f>
         <v>2.3747547154699448E-2</v>
       </c>
-      <c r="C493" t="s">
-        <v>7</v>
-      </c>
-      <c r="E493" t="s">
+      <c r="C494" t="s">
+        <v>7</v>
+      </c>
+      <c r="E494" t="s">
         <v>21</v>
       </c>
-      <c r="F493" t="s">
-        <v>19</v>
-      </c>
-      <c r="G493" t="s">
+      <c r="F494" t="s">
+        <v>19</v>
+      </c>
+      <c r="G494" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="494" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A494" s="3" t="s">
+    <row r="495" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A495" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B494" s="5">
+      <c r="B495" s="5">
         <f>0.085/24.971</f>
         <v>3.4039485803532099E-3</v>
       </c>
-      <c r="C494" t="s">
-        <v>7</v>
-      </c>
-      <c r="E494" t="s">
+      <c r="C495" t="s">
+        <v>7</v>
+      </c>
+      <c r="E495" t="s">
         <v>21</v>
       </c>
-      <c r="F494" t="s">
-        <v>19</v>
-      </c>
-      <c r="G494" t="s">
+      <c r="F495" t="s">
+        <v>19</v>
+      </c>
+      <c r="G495" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="495" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
+    <row r="496" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
         <v>245</v>
       </c>
-      <c r="B495" s="6">
+      <c r="B496" s="6">
         <f>2.75/24.971</f>
         <v>0.11012774818789796</v>
       </c>
-      <c r="C495" t="s">
-        <v>7</v>
-      </c>
-      <c r="E495" t="s">
+      <c r="C496" t="s">
+        <v>7</v>
+      </c>
+      <c r="E496" t="s">
         <v>21</v>
       </c>
-      <c r="F495" t="s">
-        <v>19</v>
-      </c>
-      <c r="G495" t="s">
+      <c r="F496" t="s">
+        <v>19</v>
+      </c>
+      <c r="G496" t="s">
         <v>246</v>
       </c>
-      <c r="I495" s="7"/>
-      <c r="J495" s="8"/>
-      <c r="K495" s="8"/>
-    </row>
-    <row r="496" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
+      <c r="I496" s="7"/>
+      <c r="J496" s="8"/>
+      <c r="K496" s="8"/>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
         <v>247</v>
       </c>
-      <c r="B496" s="6">
+      <c r="B497" s="6">
         <f>2.5/24.971</f>
         <v>0.10011613471627087</v>
       </c>
-      <c r="C496" t="s">
-        <v>7</v>
-      </c>
-      <c r="E496" t="s">
+      <c r="C497" t="s">
+        <v>7</v>
+      </c>
+      <c r="E497" t="s">
         <v>21</v>
       </c>
-      <c r="F496" t="s">
-        <v>19</v>
-      </c>
-      <c r="G496" t="s">
+      <c r="F497" t="s">
+        <v>19</v>
+      </c>
+      <c r="G497" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A497" t="s">
+    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
         <v>248</v>
       </c>
-      <c r="B497" s="6">
+      <c r="B498" s="6">
         <f>2.75/24.971</f>
         <v>0.11012774818789796</v>
       </c>
-      <c r="C497" t="s">
-        <v>7</v>
-      </c>
-      <c r="E497" t="s">
+      <c r="C498" t="s">
+        <v>7</v>
+      </c>
+      <c r="E498" t="s">
         <v>21</v>
       </c>
-      <c r="F497" t="s">
-        <v>19</v>
-      </c>
-      <c r="G497" t="s">
+      <c r="F498" t="s">
+        <v>19</v>
+      </c>
+      <c r="G498" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A498" t="s">
+    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
         <v>250</v>
       </c>
-      <c r="B498" s="9">
+      <c r="B499" s="9">
         <f>2.5/24.971</f>
         <v>0.10011613471627087</v>
       </c>
-      <c r="C498" t="s">
-        <v>7</v>
-      </c>
-      <c r="E498" t="s">
+      <c r="C499" t="s">
+        <v>7</v>
+      </c>
+      <c r="E499" t="s">
         <v>21</v>
       </c>
-      <c r="F498" t="s">
-        <v>19</v>
-      </c>
-      <c r="G498" t="s">
+      <c r="F499" t="s">
+        <v>19</v>
+      </c>
+      <c r="G499" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B499" s="10"/>
-    </row>
-    <row r="500" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A500" s="2" t="s">
+    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B500" s="10"/>
+    </row>
+    <row r="501" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A501" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B500" s="2" t="s">
+      <c r="B501" s="2" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A501" t="s">
-        <v>2</v>
-      </c>
-      <c r="B501" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="502" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B502" t="s">
-        <v>21</v>
+        <v>256</v>
       </c>
     </row>
     <row r="503" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>230</v>
-      </c>
-      <c r="B503">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B503" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="504" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>5</v>
-      </c>
-      <c r="B504" t="s">
-        <v>237</v>
+        <v>230</v>
+      </c>
+      <c r="B504">
+        <v>1</v>
       </c>
     </row>
     <row r="505" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B505" t="s">
-        <v>7</v>
+        <v>237</v>
       </c>
     </row>
     <row r="506" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
+        <v>6</v>
+      </c>
+      <c r="B506" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
         <v>216</v>
       </c>
-      <c r="B506" t="s">
+      <c r="B507" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A507" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B507" s="1"/>
-      <c r="C507" s="1"/>
-      <c r="D507" s="1"/>
-      <c r="E507" s="1"/>
-      <c r="F507" s="1"/>
-      <c r="G507" s="1"/>
     </row>
     <row r="508" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A508" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B508" s="1"/>
+      <c r="C508" s="1"/>
+      <c r="D508" s="1"/>
+      <c r="E508" s="1"/>
+      <c r="F508" s="1"/>
+      <c r="G508" s="1"/>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A509" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B508" s="1" t="s">
+      <c r="B509" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C508" s="1" t="s">
+      <c r="C509" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D508" s="1" t="s">
+      <c r="D509" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E508" s="1" t="s">
+      <c r="E509" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F508" s="1" t="s">
+      <c r="F509" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G508" s="1" t="s">
+      <c r="G509" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H508" s="1" t="s">
+      <c r="H509" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="509" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A509" s="3" t="str">
-        <f>B500</f>
+    <row r="510" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A510" s="3" t="str">
+        <f>B501</f>
         <v>market for battery, Sodium-ion, SiB</v>
-      </c>
-      <c r="B509">
-        <v>1</v>
-      </c>
-      <c r="C509" t="s">
-        <v>7</v>
-      </c>
-      <c r="E509" t="str">
-        <f>B502</f>
-        <v>GLO</v>
-      </c>
-      <c r="F509" t="s">
-        <v>18</v>
-      </c>
-      <c r="G509" t="str">
-        <f>B504</f>
-        <v>battery, SiB</v>
-      </c>
-    </row>
-    <row r="510" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A510" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="B510">
         <v>1</v>
@@ -9293,25 +9318,27 @@
       <c r="C510" t="s">
         <v>7</v>
       </c>
-      <c r="E510" t="s">
-        <v>21</v>
+      <c r="E510" t="str">
+        <f>B503</f>
+        <v>GLO</v>
       </c>
       <c r="F510" t="s">
-        <v>19</v>
-      </c>
-      <c r="G510" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A511" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="G510" t="str">
+        <f>B505</f>
+        <v>battery, SiB</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A511" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="B511">
-        <v>0.30910727700000001</v>
+        <v>1</v>
       </c>
       <c r="C511" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E511" t="s">
         <v>21</v>
@@ -9320,15 +9347,15 @@
         <v>19</v>
       </c>
       <c r="G511" t="s">
-        <v>34</v>
+        <v>254</v>
       </c>
     </row>
     <row r="512" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>231</v>
+        <v>27</v>
       </c>
       <c r="B512">
-        <v>2.4627409999999999E-2</v>
+        <v>0.30910727700000001</v>
       </c>
       <c r="C512" t="s">
         <v>24</v>
@@ -9340,15 +9367,15 @@
         <v>19</v>
       </c>
       <c r="G512" t="s">
-        <v>232</v>
+        <v>34</v>
       </c>
     </row>
     <row r="513" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B513">
-        <v>0.20877976500000001</v>
+        <v>2.4627409999999999E-2</v>
       </c>
       <c r="C513" t="s">
         <v>24</v>
@@ -9360,15 +9387,15 @@
         <v>19</v>
       </c>
       <c r="G513" t="s">
-        <v>33</v>
+        <v>232</v>
       </c>
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B514">
-        <v>0.59901584900000004</v>
+        <v>0.20877976500000001</v>
       </c>
       <c r="C514" t="s">
         <v>24</v>
@@ -9380,14 +9407,34 @@
         <v>19</v>
       </c>
       <c r="G514" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="515" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>234</v>
+      </c>
+      <c r="B515">
+        <v>0.59901584900000004</v>
+      </c>
+      <c r="C515" t="s">
+        <v>24</v>
+      </c>
+      <c r="E515" t="s">
+        <v>21</v>
+      </c>
+      <c r="F515" t="s">
+        <v>19</v>
+      </c>
+      <c r="G515" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="515" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A515" s="3"/>
+    <row r="516" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A516" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K479" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K480" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>